<commit_message>
Additional processing of the URL field is empty
</commit_message>
<xml_diff>
--- a/Extract_IP_from_URL_in_Excel/提取IP测试工作簿.xlsx
+++ b/Extract_IP_from_URL_in_Excel/提取IP测试工作簿.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B08FD316-E342-4263-A774-E68389E664D6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5197E31B-4465-48B0-8977-E3245EE7DAC6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6710" yWindow="2750" windowWidth="28800" windowHeight="15560" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13425" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="咕咕咕" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
   <si>
     <t>业务系统</t>
   </si>
@@ -65,6 +65,9 @@
     <t>奶牛产奶管理系统</t>
   </si>
   <si>
+    <t>http://ah.ssi.996icu.net:8082</t>
+  </si>
+  <si>
     <t>办公OA</t>
   </si>
   <si>
@@ -83,25 +86,23 @@
     <t>https://123.256.23.5:4433/23index.html</t>
   </si>
   <si>
-    <t>http://ah.ssi.996icu.net:8082</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <t>哇嘎嘎URL是空的系统</t>
+  </si>
+  <si>
+    <t>啦啦啦</t>
+  </si>
+  <si>
+    <t>https://192.111.23.56</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="等线"/>
-      <family val="2"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="9"/>
       <name val="等线"/>
       <family val="2"/>
       <charset val="134"/>
@@ -138,25 +139,22 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -474,20 +472,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C10"/>
+  <dimension ref="A1:C12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="13.9" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="18.25" style="4" customWidth="1"/>
-    <col min="2" max="2" width="34.58203125" style="4" customWidth="1"/>
-    <col min="3" max="3" width="25.9140625" style="4" customWidth="1"/>
+    <col min="1" max="1" width="20.265625" style="3" customWidth="1"/>
+    <col min="2" max="2" width="34.59765625" style="3" customWidth="1"/>
+    <col min="3" max="3" width="25.9296875" style="3" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -498,7 +496,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -507,7 +505,7 @@
       </c>
       <c r="C2" s="2"/>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -516,7 +514,7 @@
       </c>
       <c r="C3" s="2"/>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -525,7 +523,7 @@
       </c>
       <c r="C4" s="2"/>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A5" t="s">
         <v>9</v>
       </c>
@@ -534,7 +532,7 @@
       </c>
       <c r="C5" s="2"/>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A6" t="s">
         <v>11</v>
       </c>
@@ -543,44 +541,57 @@
       </c>
       <c r="C6" s="2"/>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A7" t="s">
         <v>13</v>
       </c>
-      <c r="B7" s="5" t="s">
+      <c r="B7" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C7" s="2"/>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A8" t="s">
+        <v>15</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C8" s="2"/>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A9" t="s">
+        <v>17</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C9" s="2"/>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A10" t="s">
+        <v>19</v>
+      </c>
+      <c r="B10" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C7" s="2"/>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
-        <v>14</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="C8" s="2"/>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
-        <v>16</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="C9" s="2"/>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
-        <v>18</v>
-      </c>
-      <c r="B10" s="3" t="s">
-        <v>19</v>
-      </c>
       <c r="C10"/>
     </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A11" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A12" t="s">
+        <v>22</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="C12"/>
+    </row>
   </sheetData>
-  <phoneticPr fontId="1" type="noConversion"/>
   <hyperlinks>
     <hyperlink ref="B2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
     <hyperlink ref="B3" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
@@ -589,9 +600,10 @@
     <hyperlink ref="B7" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
     <hyperlink ref="B9" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
     <hyperlink ref="B10" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
+    <hyperlink ref="B12" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId8"/>
+  <pageSetup paperSize="9" orientation="portrait"/>
 </worksheet>
 </file>
 
@@ -603,9 +615,8 @@
       <selection activeCell="J35" sqref="J35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="13.9" x14ac:dyDescent="0.4"/>
   <sheetData/>
-  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Support to convert domain name URL to IP address
</commit_message>
<xml_diff>
--- a/Extract_IP_from_URL_in_Excel/提取IP测试工作簿.xlsx
+++ b/Extract_IP_from_URL_in_Excel/提取IP测试工作簿.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5197E31B-4465-48B0-8977-E3245EE7DAC6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EAAD0377-E7D9-4E61-AA28-DB19FFA69523}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13425" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -65,25 +65,26 @@
     <t>奶牛产奶管理系统</t>
   </si>
   <si>
-    <t>http://ah.ssi.996icu.net:8082</t>
+    <t>http://www.bilibili.com:8082</t>
   </si>
   <si>
     <t>办公OA</t>
   </si>
   <si>
-    <t>ah.hahah.com</t>
+    <t>www.acfun.cn</t>
   </si>
   <si>
     <t>ERP</t>
   </si>
   <si>
-    <t>http://192.168.50.234:8088/os/abc</t>
+    <t>http://192.168.50.234:8088/os/abc
+http://182.78.76.234:8081/os/abc</t>
   </si>
   <si>
     <t>OBS后台系统</t>
   </si>
   <si>
-    <t>https://123.256.23.5:4433/23index.html</t>
+    <t>https://123.251.23.5:4433/23index.html</t>
   </si>
   <si>
     <t>哇嘎嘎URL是空的系统</t>
@@ -143,7 +144,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -154,6 +155,12 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -474,8 +481,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.9" x14ac:dyDescent="0.4"/>
@@ -545,34 +552,34 @@
       <c r="A7" t="s">
         <v>13</v>
       </c>
-      <c r="B7" s="4" t="s">
+      <c r="B7" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="C7" s="2"/>
+      <c r="C7" s="4"/>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A8" t="s">
         <v>15</v>
       </c>
-      <c r="B8" s="2" t="s">
+      <c r="B8" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="C8" s="2"/>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="C8" s="4"/>
+    </row>
+    <row r="9" spans="1:3" ht="27.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A9" t="s">
         <v>17</v>
       </c>
-      <c r="B9" s="1" t="s">
+      <c r="B9" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="C9" s="2"/>
+      <c r="C9" s="4"/>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A10" t="s">
         <v>19</v>
       </c>
-      <c r="B10" s="4" t="s">
+      <c r="B10" s="6" t="s">
         <v>20</v>
       </c>
       <c r="C10"/>
@@ -586,7 +593,7 @@
       <c r="A12" t="s">
         <v>22</v>
       </c>
-      <c r="B12" s="4" t="s">
+      <c r="B12" s="6" t="s">
         <v>23</v>
       </c>
       <c r="C12"/>
@@ -598,9 +605,10 @@
     <hyperlink ref="B4" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
     <hyperlink ref="B6" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
     <hyperlink ref="B7" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
-    <hyperlink ref="B9" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
-    <hyperlink ref="B10" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
-    <hyperlink ref="B12" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
+    <hyperlink ref="B8" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
+    <hyperlink ref="B9" r:id="rId7" display="http://192.168.50.234:8088/os/abc" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
+    <hyperlink ref="B10" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
+    <hyperlink ref="B12" r:id="rId9" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>

</xml_diff>